<commit_message>
descw-1267 finish excel report and tweak model for readability
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_32_rpt_PA_Registered.xlsx
+++ b/backend/reports/xlsx/Tab_32_rpt_PA_Registered.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2D95-0CAF-9C4E-86F6-F58748A44EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4E77B0-A148-3648-8056-083F2BD7CBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -59,7 +50,98 @@
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Projects Registered on or after {$afterDate}</t>
+  </si>
+  <si>
+    <t>{#row=d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#rows=d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>{#p=d.report[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{#p1=d.report[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{#subtotals=d.report[i].portfolio_totals}</t>
+  </si>
+  <si>
+    <t>{#subtotals1=d.report[i].subtotals}</t>
+  </si>
+  <si>
+    <t>{#grandTotals=d.grand_totals}</t>
+  </si>
+  <si>
+    <t>{#afterDate=d.afterDate}</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Registration
+Date</t>
+  </si>
+  <si>
+    <t>Start
+Date</t>
+  </si>
+  <si>
+    <t>End
+Date</t>
+  </si>
+  <si>
+    <t>Planned
+Budget</t>
+  </si>
+  <si>
+    <t>Ministry</t>
+  </si>
+  <si>
+    <t>Report Total: {$grandTotals.total}</t>
+  </si>
+  <si>
+    <t>{$p.project_manager}</t>
+  </si>
+  <si>
+    <t>{$p.description}</t>
+  </si>
+  <si>
+    <t>{$p.initiation_date}</t>
+  </si>
+  <si>
+    <t>{$p.start_date}</t>
+  </si>
+  <si>
+    <t>{$p.end_date}</t>
+  </si>
+  <si>
+    <t>{$p.planned_budget}</t>
+  </si>
+  <si>
+    <t>{$p.ministry}</t>
+  </si>
+  <si>
+    <t>{$p1}</t>
+  </si>
+  <si>
+    <t>{$p.#}</t>
+  </si>
+  <si>
+    <t>{$p.name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {$rows.portfolio_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {$row.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$row.portfolio_name} Total:{$subtotals.total}</t>
   </si>
 </sst>
 </file>
@@ -69,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,31 +164,40 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="7.5"/>
+      <color rgb="FF000000"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,28 +216,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -197,54 +285,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,6 +477,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFBFBF"/>
+      <color rgb="FFF1F2F2"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -623,112 +849,228 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B12"/>
+      <selection activeCell="C15" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="5" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="41" thickBot="1">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="20" thickTop="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="20" thickTop="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="19">
-      <c r="B7" s="16" t="s">
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="7"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19">
-      <c r="B8" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="19">
-      <c r="B9" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="19">
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="19">
-      <c r="B11" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="19">
-      <c r="B12" s="16" t="s">
-        <v>3</v>
+    <row r="22" spans="2:6">
+      <c r="B22" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>